<commit_message>
Added feature where a user can supply their own cutoffs for the plots
</commit_message>
<xml_diff>
--- a/data/Man_Input_Cutoff_test.xlsx
+++ b/data/Man_Input_Cutoff_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4D860D7-B4F7-7B4B-B594-F7B7636E9A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABBEA9D-6712-8041-8697-00D6CD58F070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="5060" windowWidth="28040" windowHeight="16940" xr2:uid="{A2ADDA60-11E9-414E-A7A9-57B6211DC17B}"/>
+    <workbookView xWindow="480" yWindow="1060" windowWidth="28040" windowHeight="16940" xr2:uid="{A2ADDA60-11E9-414E-A7A9-57B6211DC17B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,40 +44,40 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Sequencing_depth</t>
-  </si>
-  <si>
-    <t>Trimming</t>
-  </si>
-  <si>
-    <t>Alignment</t>
-  </si>
-  <si>
-    <t>Ribosomal_RNA</t>
-  </si>
-  <si>
-    <t>Gene_exon_mapping</t>
-  </si>
-  <si>
     <t>GeneBody_Coverage</t>
   </si>
   <si>
     <t>Dist_of_gene_expression</t>
   </si>
   <si>
-    <t>Sequence_contamination_overrep_pretrim</t>
-  </si>
-  <si>
-    <t>Sequence_contamination_adapter_pretrim</t>
-  </si>
-  <si>
-    <t>Sequence_contamination_adapter_posttrim</t>
-  </si>
-  <si>
-    <t>Sequence_contamination_overrep_posttrim</t>
-  </si>
-  <si>
     <t>cutoff</t>
+  </si>
+  <si>
+    <t>_ipReads_cutoff</t>
+  </si>
+  <si>
+    <t>_trimmedReads_cutoff</t>
+  </si>
+  <si>
+    <t>_uniqAligned_cutoff</t>
+  </si>
+  <si>
+    <t>_exonMapping_cutoff</t>
+  </si>
+  <si>
+    <t>_riboScatter_cutoff</t>
+  </si>
+  <si>
+    <t>_violin_cutoff_overrep_untrimmed</t>
+  </si>
+  <si>
+    <t>_violin_cutoff_overrep_trimmed</t>
+  </si>
+  <si>
+    <t>_violin_cutoff_adapter_untrimmed</t>
+  </si>
+  <si>
+    <t>_violin_cutoff_adapter_trimmed</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A80B42A-D43C-EF42-AB3C-2241D6BE208E}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -440,7 +442,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -451,7 +453,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -462,7 +464,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>80</v>
@@ -473,7 +475,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -484,7 +486,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -495,12 +497,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -511,7 +513,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -522,7 +524,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -533,7 +535,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -544,7 +546,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>0.05</v>
@@ -555,7 +557,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>0.05</v>

</xml_diff>